<commit_message>
Improve table styling in save_to_files function
</commit_message>
<xml_diff>
--- a/output/Amazon.xlsx
+++ b/output/Amazon.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>Nombre</t>
   </si>
@@ -22,58 +22,58 @@
     <t>Precio</t>
   </si>
   <si>
-    <t>Computadora portátil, pantalla IPS FHD de 15.6 pulgadas (1920 x 1080), Intel Core i3-5005U, 16 GB de RAM y 512 GB SSD portátil, WiFi 2.4G/5G, BT5.0 y RJ45, completamente funcional tipo C, gris</t>
-  </si>
-  <si>
-    <t>Nimo Portátil estudiantil 15.6 FHD, 16 GB de RAM, SSD de 1 TB, Intel Pentium Quad-Core N100 (Beat to i3-1115G4, hasta 3.4GHz), teclado retroiluminado, huella digital, 2 años de garantía, 90 días de</t>
+    <t>Computadora portátil Windows 11 Pro de 15.6 pulgadas, 16 GB de RAM, 1 TB NVMe SSD Intel Alder Lake-N100 de 12ª generación (hasta 3.4 GHz), computadora portátil ligera y delgada, pantalla FHD,</t>
+  </si>
+  <si>
+    <t>ACEMAGIC Computadora portátil Pantalla FHD de 15.6 pulgadas, 16 GB de RAM 512 GB de ROM con Intel N95 de cuatro núcleos (4C/4T, hasta 3.4 GHz), Windows 11, soporte para portátil WiFi, BT5.0, cámara</t>
   </si>
   <si>
     <t>Lenovo IdeaPad 1 - Laptop con pantalla FHD de 15.6 pulgadas, AMD Ryzen 5 5500U, 8 GB de RAM, SSD de 512 GB, Windows 11 Home, cámara de 720p con obturador de privacidad, cancelación inteligente de</t>
   </si>
   <si>
+    <t>HP Laptop ultraligera de 14 pulgadas para estudiantes y negocios, Intel Quad-Core N4120, 8 GB de RAM, 192 GB de almacenamiento (64 GB eMMC + 128 GB Micro SD), 1 año Office 365, cámara web, HDMI, WiFi,</t>
+  </si>
+  <si>
     <t>ASUS Portátil Vivobook Go de 15,6", Intel Celeron N4500, 4 GB de RAM, SSD de 128 GB, Windows 11 en modo S, negro estrella, L510KA-ES04</t>
   </si>
   <si>
+    <t>HP Computadora portátil 14, Intel Celeron N4020, 4 GB de RAM, 64 GB de almacenamiento, pantalla HD de microborde de 14 pulgadas, Windows 11 Home, delgada y portátil, gráficos 4K, un año de Microsoft</t>
+  </si>
+  <si>
+    <t>ANMESC Computadora portátil, 16 GB de RAM 512 GB ROM Intel Celeron Quad-Core, 15.6 pulgadas Laptops, 1920 x 1080 IPS, 38Wh Batería, WiFi, Bluetooth, Tipo-C, Tarjeta TF, Mini-HDMI</t>
+  </si>
+  <si>
+    <t>Acer Aspire Go 15 Slim Laptop | FHD de 15.6 pulgadas (1920 x 1080) IPS | Intel Core i3-N305 | Gráficos Intel UHD | 8 GB LPDDR5 | 128GB HD | Wi-Fi 6 | PC AI| Windows 11 Home en modo S | AG15-31P-3947</t>
+  </si>
+  <si>
+    <t>HP Computadora portátil 17, pantalla HD+ de 17.3", procesador Intel Core i3-1125G4 de 11ª generación, 32 GB de RAM, SSD de 1 TB, Wi-Fi, HDMI, cámara web, Windows 11 Home, color plateado</t>
+  </si>
+  <si>
     <t>Laptop de 15.6 pulgadas, 8 GB DDR4 256 GB SSD, computadora portátil con procesador Celeron N4000 (hasta 2.6 GHz), mini HDMI, USB 3.2, WiFi dual, tipo C, 7000 mAh, teclado numérico, cámara web</t>
   </si>
   <si>
-    <t>HP Laptop ultraligera de 14 pulgadas para estudiantes y negocios, Intel Quad-Core N4120, 8 GB de RAM, 192 GB de almacenamiento (64 GB eMMC + 128 GB Micro SD), 1 año Office 365, cámara web, HDMI, WiFi,</t>
-  </si>
-  <si>
-    <t>ACEMAGIC Computadora portátil Pantalla FHD de 15.6 pulgadas, 16 GB de RAM 512 GB de ROM con Intel N95 de cuatro núcleos (4C/4T, hasta 3.4 GHz), Windows 11, soporte para portátil WiFi, BT5.0, cámara</t>
-  </si>
-  <si>
-    <t>Acer Aspire Go 15 Slim Laptop | FHD de 15.6 pulgadas (1920 x 1080) IPS | Intel Core i3-N305 | Gráficos Intel UHD | 8 GB LPDDR5 | 128GB HD | Wi-Fi 6 | PC AI| Windows 11 Home en modo S | AG15-31P-3947</t>
-  </si>
-  <si>
-    <t>HP Computadora portátil 17, pantalla HD+ de 17.3", procesador Intel Core i3-1125G4 de 11ª generación, 32 GB de RAM, SSD de 1 TB, Wi-Fi, HDMI, cámara web, Windows 11 Home, color plateado</t>
-  </si>
-  <si>
-    <t>HP Computadora portátil 14, Intel Celeron N4020, 4 GB de RAM, 64 GB de almacenamiento, pantalla HD de microborde de 14 pulgadas, Windows 11 Home, delgada y portátil, gráficos 4K, un año de Microsoft</t>
-  </si>
-  <si>
     <t>Lenovo Laptop empresarial V15 | 16 GB de RAM | SSD de 1 TB | Pantalla antirreflejos FHD de 15.6 pulgadas | Procesador Intel de doble núcleo | Ethernet RJ-45 | Licencia de por vida de Microsoft Office</t>
   </si>
   <si>
-    <t>ACEMAGIC Ordenador portátil de 16 pulgadas IPS Intel N95 16GB DDR4 512GB SSD Windows Ordenador portátil tradicional FHD 1920 * 1200 Pantalla WiFi BT5.0 HDMI Tipo-C USB Oficina Portátil Portátil</t>
+    <t>LG gram Pro 2 en 1 portátil ligero y versátil de 16 pulgadas, Intel Evo Edition, Intel Core Ultra 7, 16 GB de RAM, SSD de 1 TB, color negro</t>
+  </si>
+  <si>
+    <t>ASUS Portátil ligero Full HD de 15.5", sistema operativo Windows 11 Home, procesador Intel Celeron de hasta 2.76 GHz, 4 GB LPDDR4, SSD de 128 GB, teclado retroiluminado, gris oscuro (renovado)</t>
   </si>
   <si>
     <t>HP Portátil portátil, pantalla táctil HD de 15.6", procesador Intel Core i3-1115G4, 32 GB de RAM, SSD PCIe de 1 TB, cámara web, tipo C, HDMI, lector de tarjetas SD, Wi-Fi, Windows 11 Home, color</t>
   </si>
   <si>
-    <t>HP Stream - Laptop BrightView HD de 14 pulgadas, Intel Celeron N4120, 16 GB de RAM, 288 GB de almacenamiento (128 GB Emmc+ 160 GB de estación de acoplamiento), gráficos Intel UHD, cámara web 720p,</t>
+    <t>HP Laptop portátil de 15.6 pulgadas (incluye Microsoft 365 de 1 año), pantalla HD, procesador Intel Quad-Core N200, 16 GB de RAM, 128 GB de almacenamiento, Wi-Fi 5, cámara web, HDMI, teclado numérico,</t>
   </si>
   <si>
     <t>Laptop HP HD de 14 pulgadas, Windows 11, procesador Intel Celeron de doble núcleo hasta 2.60 GHz, 4 GB de RAM, 64 GB SSD, cámara web, rosa Dale (renovado) (azul dale)</t>
   </si>
   <si>
-    <t>HP Portátil portátil, estudiante y empresarial, pantalla HD de 14", Intel Quad-Core N4120, 8GB DDR4 RAM, 64GB eMMC, 1 año Office 365, cámara web, RJ-45, HDMI, Wi-Fi, Windows 11 Home, plata</t>
-  </si>
-  <si>
-    <t>ASUS Portátil ligero Full HD de 15.5", sistema operativo Windows 11 Home, procesador Intel Celeron de hasta 2.76 GHz, 4 GB LPDDR4, SSD de 128 GB, teclado retroiluminado, gris oscuro (renovado)</t>
-  </si>
-  <si>
-    <t>HP Laptop portátil de 15.6 pulgadas (incluye Microsoft 365 de 1 año), pantalla HD, procesador Intel Quad-Core N200, 16 GB de RAM, 128 GB de almacenamiento, Wi-Fi 5, cámara web, HDMI, teclado numérico,</t>
+    <t>jumper Computadora portátil, 12 GB LPDDR4 RAM, 512 GB SSD ROM, pantalla IPS FHD de 14 pulgadas 1080p, computadora portátil Windows 11 con procesador Celeron Quad-Core, gráficos UHD 600, altavoz</t>
+  </si>
+  <si>
+    <t>HP Stream - Portátil ligero HD de 14 pulgadas, Intel Celeron N4120, 16 GB de RAM, 192 GB de almacenamiento (64 GB eMMC + tarjeta USB de 128 GB), gráficos Intel UHD, cámara web HD, 1 año de Office 365,</t>
   </si>
   <si>
     <t>Dell Inspiron 15 3000 3520 - Computadora portátil empresarial [Windows 11 Pro], pantalla táctil FHD de 15.6 pulgadas, Intel Quad-Core i5-1135G7 de 11ª generación, 16 GB de RAM, SSD PCIe de 1 TB,</t>
@@ -82,70 +82,112 @@
     <t>HP Computadora portátil HD de 14 pulgadas, Intel Celeron N4120, 4 GB, DDR4 RAM, 64 GB, eMMC UHD Graphics 600, teclado blanco nieve, lector de tarjetas SD, puerto HDMI para micrófono, auriculares,</t>
   </si>
   <si>
-    <t>Lenovo Ideapad 3i - Laptop con pantalla táctil FHD de 15.6 pulgadas, procesador Intel i3-1115G4, 40 GB RAM 1TB SSD, Windows 11 Pro, teclado numérico, auriculares Plusera, gris ártico, gris ártico,</t>
+    <t>ASUS Portátil IPS antirreflejo FHD de 15.5", procesador Intel Celeron N de hasta 2.79 GHz, 4 GB DDR4, 256 GB de almacenamiento, Bluetooth, teclado retroiluminado, cámara web, Windows 11, azul oscuro,</t>
+  </si>
+  <si>
+    <t>Extensor de pantalla para laptop, 14 pulgadas, FHD 1080P IPS, extensor de monitor de computadora portátil, monitor portátil para portátiles de 13 a 17 pulgadas con puerto USB-C/HDMI, Plug n</t>
+  </si>
+  <si>
+    <t>HP Stream - Laptop BrightView HD de 14 pulgadas, Intel Celeron N4120, 16 GB de RAM, 256 GB de almacenamiento (128 GB eMMC + tarjeta USB de 128 GB), gráficos Intel UHD, cámara HD, carga rápida, 1 año</t>
+  </si>
+  <si>
+    <t>ASUS C423NA Chromebook 14" HD Laptop (Intel Dual Core Celeron Processor N3350, 4GB DDR4 RAM, 64GB SSD) Webcam, WiFi, Bluetooth, Type-C, Google Chrome OS - Silver (Renewed)</t>
+  </si>
+  <si>
+    <t>HP Stream 2022, pantalla HD de 14 pulgadas, procesador Intel Celeron N4120, memoria de 4 GB, 64 GB eMMC, WiFi, Bluetooth, tipo C, 802.11AC, Win10 S, blanco copo de nieve</t>
+  </si>
+  <si>
+    <t>ASUS Vivobook F1605ZA-AS56 - Computadora portátil WUXGA de 16 pulgadas, memoria de 16 GB, SSD de 512 GB, plata fría</t>
+  </si>
+  <si>
+    <t>HP Laptop empresarial 255 G10 FHD de 15.6 pulgadas, AMD Ryzen 7 7730U, 32 GB de RAM, SSD PCIe de 1 TB, teclado numérico, cámara web, Wi-Fi 6, HDMI, Windows 11 Pro, negro</t>
+  </si>
+  <si>
+    <t>ACEMAGIC Computadora portátil de 16 pulgadas, alimentado por procesador N95, 16 GB DDR4 RAM 512 GB SSD, FHD 1920 x 1200P, tipo C, batería de 38 Wh, WiFi, BT5.0, portátil tradicional para las</t>
+  </si>
+  <si>
+    <t>ASUS Laptop Vivobook Go 2024 HD de 11.6 pulgadas, Intel Celeron N4500, gráficos Intel, 4GB, 128GB, Windows 11 Home en modo S, negro estrella, L210KA-ES04</t>
+  </si>
+  <si>
+    <t>HP Laptop HD de 14 pulgadas, Windows 11, procesador Intel Celeron de doble núcleo hasta 2.60 GHz, 4 GB de RAM, 64 GB SSD, cámara web, rosa Dale (renovado) (rosa intenso)</t>
+  </si>
+  <si>
+    <t>359</t>
+  </si>
+  <si>
+    <t>349</t>
+  </si>
+  <si>
+    <t>269</t>
+  </si>
+  <si>
+    <t>227</t>
+  </si>
+  <si>
+    <t>429</t>
+  </si>
+  <si>
+    <t>399</t>
+  </si>
+  <si>
+    <t>249</t>
+  </si>
+  <si>
+    <t>187</t>
+  </si>
+  <si>
+    <t>239</t>
+  </si>
+  <si>
+    <t>278</t>
+  </si>
+  <si>
+    <t>491</t>
+  </si>
+  <si>
+    <t>529</t>
+  </si>
+  <si>
+    <t>1,562</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>449</t>
   </si>
   <si>
     <t>299</t>
   </si>
   <si>
-    <t>329</t>
-  </si>
-  <si>
-    <t>349</t>
-  </si>
-  <si>
-    <t>227</t>
-  </si>
-  <si>
-    <t>239</t>
-  </si>
-  <si>
-    <t>399</t>
-  </si>
-  <si>
-    <t>269</t>
-  </si>
-  <si>
-    <t>359</t>
-  </si>
-  <si>
-    <t>278</t>
-  </si>
-  <si>
-    <t>491</t>
-  </si>
-  <si>
-    <t>187</t>
-  </si>
-  <si>
-    <t>529</t>
-  </si>
-  <si>
-    <t>369</t>
-  </si>
-  <si>
-    <t>449</t>
-  </si>
-  <si>
-    <t>309</t>
-  </si>
-  <si>
     <t>165</t>
   </si>
   <si>
-    <t>215</t>
-  </si>
-  <si>
-    <t>161</t>
-  </si>
-  <si>
     <t>503</t>
   </si>
   <si>
     <t>137</t>
   </si>
   <si>
-    <t>689</t>
+    <t>179</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>298</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>549</t>
+  </si>
+  <si>
+    <t>619</t>
+  </si>
+  <si>
+    <t>379</t>
   </si>
 </sst>
 </file>
@@ -163,7 +205,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -178,7 +220,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9EAD3"/>
+        <fgColor rgb="FFD0E0E3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,8 +267,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B26" totalsRowShown="0">
-  <autoFilter ref="A1:B26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B35" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Nombre"/>
     <tableColumn id="2" name="Precio"/>
@@ -520,7 +561,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -543,7 +584,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -551,7 +592,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -559,7 +600,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -567,7 +608,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -575,118 +616,115 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="B7" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -694,7 +732,7 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -702,7 +740,7 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -710,7 +748,7 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -718,7 +756,7 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -726,7 +764,76 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Examen y practicas anteriores
</commit_message>
<xml_diff>
--- a/output/Amazon.xlsx
+++ b/output/Amazon.xlsx
@@ -14,144 +14,183 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Precio</t>
-  </si>
-  <si>
-    <t>Lenovo V15 Business Laptop | 16GB RAM | 1TB SSD | 15.6"" FHD Anti-Glare Display | Intel Dual-core Processor | Ethernet RJ-45 | Microsoft Office Lifetime License | Windows 11 Pro | WOWPC Bundle, Black</t>
-  </si>
-  <si>
-    <t>HP 14" HD Laptop | Back to School Limited Edition with 1 Year Microsoft 365 | Intel Quad-Core Processor | 8GB RAM | 576GB Storage | Long Battery Life | Pink | w/WOWPC Bundle | Windows 11</t>
-  </si>
-  <si>
-    <t>Lenovo IdeaPad 1 Laptop, 15.6” FHD Display, AMD Ryzen 5 5500U, 8GB RAM, 512GB SSD, Windows 11 Home, 720p Camera w/Privacy Shutter, Smart Noise Cancelling, Cloud Grey</t>
-  </si>
-  <si>
-    <t>ASUS 15.6” Vivobook Go Laptop, Intel Celeron N4500, 4GB RAM, 128GB SSD, Windows 11 in S Mode, Star Black, L510KA-ES04</t>
-  </si>
-  <si>
-    <t>HP Newest 14" Ultral Light Laptop for Students and Business, Intel Quad-Core N4120, 8GB RAM, 192GB Storage(64GB eMMC+128GB Micro SD), 1 Year Office 365, Webcam, HDMI, WiFi, USB-A&amp;C, Win 11 S</t>
-  </si>
-  <si>
-    <t>Acer Aspire Go 15 Slim Laptop | 15.6" Full HD IPS 1080P Display | Intel Core i3-N305| Intel UHD Graphics | 8GB LPDDR5 | 128GB HD | Wi-Fi 6 | AI PC | Windows 11 Home in S Mode | AG15-31P-3947</t>
-  </si>
-  <si>
-    <t>HP 255 G8 Portable Laptop, Business and Professional, 15.6" FHD Display, AMD Ryzen 5 5500U, 32GB RAM, 2TB PCIe SSD, Webcam, SD Card Reader, HDMI, Wi-Fi 6, Windows 11 Pro, Dark Ash Silver</t>
-  </si>
-  <si>
-    <t>HP 14 Laptop, Intel Celeron N4020, 4 GB RAM, 64 GB Storage, 14-inch Micro-edge HD Display, Windows 11 Home, Thin &amp; Portable, 4K Graphics, One Year of Microsoft 365 (14-dq0040nr, Snowflake White)</t>
-  </si>
-  <si>
-    <t>HP 17 Laptop, 17.3” HD+ Display, 11th Gen Intel Core i3-1125G4 Processor, 32GB RAM, 1TB SSD, Wi-Fi, HDMI, Webcam, Windows 11 Home, Silver</t>
-  </si>
-  <si>
-    <t>HP Portable Laptop, Student and Business, 14" HD Display, Intel Quad-Core N4120, 8GB DDR4 RAM, 64GB eMMC, 1 Year Office 365, Webcam, RJ-45, HDMI, Wi-Fi, Windows 11 Home, Silver</t>
-  </si>
-  <si>
-    <t>HP Notebook Laptop, 15.6" HD Touchscreen, Intel Core i3-1115G4 Processor, 32GB RAM, 1TB PCIe SSD, Webcam, Type-C, HDMI, SD Card Reader, Wi-Fi, Windows 11 Home, Silver</t>
-  </si>
-  <si>
-    <t>HP Victus 15.6 inch Laptop, FHD 144Hz Display, Intel Core i5-12450H, 8 GB RAM, 512 GB SSD, NVIDIA GeForce RTX 2050 GPU (4 GB Dedicated), Windows 11 Home, 15-fa1029nr (2024)</t>
-  </si>
-  <si>
-    <t>Lenovo V-Series V15 Business Laptop, 15.6" FHD Display, AMD Ryzen 7 7730U, 40GB RAM, 1TB SSD, Numeric Keypad, HDMI, RJ45, Webcam, Wi-Fi 6, Windows 11 Pro, Black</t>
-  </si>
-  <si>
-    <t>15.6 Inch Laptop, 8GB DDR4 256GB SSD, Laptops Computer with Celeron N4000 Processor(up to 2.6GHz), Mini HDMI, USB3.2, Dual WiFi, Type-C, 7000mAh, Numeric Keypad, Webcam(Sliver)</t>
-  </si>
-  <si>
-    <t>HP 15.6" Portable Laptop (Include 1 Year Microsoft 365), HD Display, Intel Quad-Core N200 Processor, 16GB RAM, 128GB Storage, Wi-Fi 5, Webcam, HDMI, Numeric Keypad, Windows 11 Home, Red</t>
-  </si>
-  <si>
-    <t>Newest HP 14" HD Laptop, Windows 11, Intel Celeron Dual-Core Processor Up to 2.60GHz, 4GB RAM, 64GB SSD, Webcam, Dale Pink(Renewed) (Dale Blue)</t>
-  </si>
-  <si>
-    <t>HP Stream 14" HD BrightView Laptop, Intel Celeron N4120, 16GB RAM, 256GB Storage (128GB eMMC + 128GB USB Card), Intel UHD Graphics, HD Camera, Fast Charge, 1 Year Office 365, Win 11 S, Gold</t>
-  </si>
-  <si>
-    <t>Lenovo IdeaPad 1 Student Laptop, Intel Dual Core Processor, 20GB RAM, 1TB SSD + 128GB eMMC, 15.6" FHD Display, 1 Year Office 365, Windows 11 Home, Wi-Fi 6, Webcam, Bluetooth, SD Card Reader, Grey</t>
-  </si>
-  <si>
-    <t>HP Stream 14" HD Lightweight Laptop, Intel Celeron N4120, 16GB RAM, 224GB Storage(64GB eMMC + 160GB Docking Station), Intel UHD Graphics, HD Webcam, 1 Year Office 365, WiFi, Bluetooth, Win 11s, Pink</t>
-  </si>
-  <si>
-    <t>ASUS Lightweight 15.5" Full HD Laptop, Windows 11 Home OS, Intel Celeron Processor Up to 2.76GHz, 4GB LPDDR4, 128GB SSD, Backlit Keyboard, Dark Gray (Renewed)</t>
-  </si>
-  <si>
-    <t>HP 2022 Newest Stream 14" HD Display, Intel Celeron N4120 Processor, 4GB Memory - 64GB eMMC,WiFi,Bluetooth, Type-C, 802.11AC, Win10 S - Snowflake White</t>
-  </si>
-  <si>
-    <t>Lenovo Newest V15 Gen 4 Laptop, 15.6" FHD Display, Intel Core i5-13420H (Beat i7-1355U), 40GB RAM, 1TB SSD, HDMI, RJ45, Numeric Keypad, Webcam, Wi-Fi, Windows 11 Home, Black</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Computadora portátil, 16 GB LPDDR5 RAM Laptop 512 GB NVMe SSD, procesador N100 de 4 núcleos, pantalla IPS de 15.6 pulgadas 1080P Win11 Pro, WiFi 6, BT 5.0, RJ45 Ethernet, USB tipo C, huella</t>
+  </si>
+  <si>
+    <t>Lenovo Ideapad - Laptop FHD Essential de 15.6 pulgadas, procesador Intel 12ª generación 6-Core i3 (hasta 4.4 GHz, Beat i5-1155G7), 24 GB de RAM, SSD de 1 TB, cámara web, Bluetooth, Wi-Fi 6, Win 11,</t>
+  </si>
+  <si>
+    <t>Lenovo IdeaPad 1 - Laptop con pantalla FHD de 15.6 pulgadas, AMD Ryzen 5 5500U, 8 GB de RAM, SSD de 512 GB, Windows 11 Home, cámara de 720p con obturador de privacidad, cancelación inteligente de</t>
+  </si>
+  <si>
+    <t>ASUS Portátil Vivobook Go de 15,6", Intel Celeron N4500, 4 GB de RAM, SSD de 128 GB, Windows 11 en modo S, negro estrella, L510KA-ES04</t>
+  </si>
+  <si>
+    <t>HP Laptop ultraligera de 14 pulgadas para estudiantes y negocios, Intel Quad-Core N4120, 8 GB de RAM, 192 GB de almacenamiento (64 GB eMMC + 128 GB Micro SD), 1 año Office 365, cámara web, HDMI, WiFi,</t>
+  </si>
+  <si>
+    <t>Acer Aspire Go 15 Slim Laptop | FHD de 15.6 pulgadas (1920 x 1080) IPS | Intel Core i3-N305 | Gráficos Intel UHD | 8 GB LPDDR5 | 128GB HD | Wi-Fi 6 | PC AI| Windows 11 Home en modo S | AG15-31P-3947</t>
+  </si>
+  <si>
+    <t>Lenovo Laptop de 15.6 pulgadas, procesador Intel Pentium de 4 núcleos, pantalla antirreflejos FHD de 15.6 pulgadas, puerto Ethernet, HDMI, USB-C, WiFi y Bluetooth, cámara web (Windows 11 Home, 40 GB</t>
+  </si>
+  <si>
+    <t>HP Computadora portátil 14, Intel Celeron N4020, 4 GB de RAM, 64 GB de almacenamiento, pantalla HD de microborde de 14 pulgadas, Windows 11 Home, delgada y portátil, gráficos 4K, un año de Microsoft</t>
+  </si>
+  <si>
+    <t>HP Portátil portátil, estudiante y empresarial, pantalla HD de 14", Intel Quad-Core N4120, 8GB DDR4 RAM, 64GB eMMC, 1 año Office 365, cámara web, RJ-45, HDMI, Wi-Fi, Windows 11 Home, plata</t>
+  </si>
+  <si>
+    <t>Laptop HP HD de 14 pulgadas, Windows 11, procesador Intel Celeron de doble núcleo hasta 2.60 GHz, 4 GB de RAM, 64 GB SSD, cámara web, rosa Dale (renovado) (azul dale)</t>
+  </si>
+  <si>
+    <t>HP Stream - Laptop BrightView HD de 14 pulgadas, Intel Celeron N4120, 16 GB de RAM, 288 GB de almacenamiento (128 GB Emmc+ 160 GB de estación de acoplamiento), gráficos Intel UHD, cámara web 720p,</t>
+  </si>
+  <si>
+    <t>Computadora portátil de 16 pulgadas, portátil para juegos, 16 GB de RAM 512 GB SSD, procesador Intel N95 de 12ª generación (hasta 3.4 GHz), FHD 1920 x 1200, apertura de ángulo de 180,</t>
+  </si>
+  <si>
+    <t>AOC Computadora portátil con pantalla FHD de 15.6 pulgadas con procesador N97 (hasta 3.6 GHz) 16 GB de RAM 512 GB SSD, portátiles para juegos, Windows 11, computadora portátil, ligera y delgada,</t>
+  </si>
+  <si>
+    <t>Lenovo Laptop empresarial V15 | 16 GB de RAM | SSD de 1 TB | Pantalla antirreflejos FHD de 15.6 pulgadas | Procesador Intel de doble núcleo | Ethernet RJ-45 | Licencia de por vida de Microsoft Office</t>
+  </si>
+  <si>
+    <t>Laptop de 15.6 pulgadas, 8 GB DDR4 256 GB SSD, computadora portátil con procesador Celeron N4000 (hasta 2.6 GHz), mini HDMI, USB 3.2, WiFi dual, tipo C, 7000 mAh, teclado numérico, cámara web</t>
+  </si>
+  <si>
+    <t>ASUS Portátil ligero Full HD de 15.5", sistema operativo Windows 11 Home, procesador Intel Celeron de hasta 2.76 GHz, 4 GB LPDDR4, SSD de 128 GB, teclado retroiluminado, gris oscuro (renovado)</t>
+  </si>
+  <si>
+    <t>HP Laptop portátil de 15.6 pulgadas (incluye Microsoft 365 de 1 año), pantalla HD, procesador Intel Quad-Core N200, 16 GB de RAM, 128 GB de almacenamiento, Wi-Fi 5, cámara web, HDMI, teclado numérico,</t>
+  </si>
+  <si>
+    <t>Portátil Pro de 16 pulgadas, 32 GB de RAM y SSD de 1 TB, Core i5-1035G4, BaseBook Pro para juegos ligeros y producción, 16:10,1200P IPS, 100% sRGB, puerto LAN, huella digital, plata</t>
+  </si>
+  <si>
+    <t>Laptops de 17.3 pulgadas, computadora portátil, 8 GB de RAM 256 GB de ROM, procesador Celeron Quad-core (hasta 2.4 GHz), WiFi 5G, cámara web, mini HDMI, 8000mAh, tipo C, 2 USB 3.2, BT5.0,</t>
+  </si>
+  <si>
+    <t>HP Portátil portátil, pantalla táctil HD de 15.6", procesador Intel Core i3-1115G4, 32 GB de RAM, SSD PCIe de 1 TB, cámara web, tipo C, HDMI, lector de tarjetas SD, Wi-Fi, Windows 11 Home, color</t>
+  </si>
+  <si>
+    <t>HP Stream - Laptop BrightView HD de 14 pulgadas, Intel Celeron N4120, 16 GB de RAM, 256 GB de almacenamiento (128 GB eMMC + tarjeta USB de 128 GB), gráficos Intel UHD, cámara HD, carga rápida, 1 año</t>
+  </si>
+  <si>
+    <t>Dell Inspiron 15 3000 3520 - Computadora portátil empresarial [Windows 11 Pro], pantalla táctil FHD de 15.6 pulgadas, Intel Quad-Core i5-1135G7 de 11ª generación, 16 GB de RAM, SSD PCIe de 1 TB,</t>
+  </si>
+  <si>
+    <t>Lenovo Ideapad 3i - Laptop con pantalla táctil FHD de 15.6 pulgadas, procesador Intel i3-1115G4, 40 GB RAM 1TB SSD, Windows 11 Pro, teclado numérico, auriculares Plusera, gris ártico, gris ártico,</t>
+  </si>
+  <si>
+    <t>Lenovo Laptop FHD de 15.6 pulgadas, procesador Intel Pentium N6000 de cuatro núcleos, memoria de 16 GB, almacenamiento SSD de 1 TB, puerto Ethernet, HDMI, USB-C, WiFi y Bluetooth, Windows 11 Home,</t>
+  </si>
+  <si>
+    <t>HP Portátil de negocios 17, pantalla HD+ de 17.3", procesador Intel Core i3-1125G4 de 11ª generación, 32 GB de RAM, SSD de 1 TB, Wi-Fi, HDMI, cámara web, Windows 11 Pro, color plateado</t>
+  </si>
+  <si>
+    <t>HP Laptop HD de 14 pulgadas, Windows 11, procesador Intel Celeron de doble núcleo hasta 2.60 GHz, 4 GB de RAM, 64 GB SSD, cámara web, rosa Dale (renovado) (rosa intenso)</t>
+  </si>
+  <si>
+    <t>ASUS Portátil para juegos ROG Strix G16 (2024), pantalla FHD 16:10 de 16 pulgadas, 165 Hz, NVIDIA® GeForce RTX™ 4060, Intel Core i7-13650HX, DDR5 de 16 GB, SSD PCIe Gen4 de 1 TB, Wi-Fi 6E, Windows 11,</t>
+  </si>
+  <si>
+    <t>acer Chromebook 2024, pantalla HD IPS ComfyView de 15 pulgadas, procesador Intel Celeron N de hasta 2.70 GHz, 4 GB LPDDR4, 64 GB eMMC, gráficos Intel UHD, WiFi de 6ª generación, cámara web, Chrome OS,</t>
+  </si>
+  <si>
+    <t>ASUS Portátil IPS antirreflejo FHD de 15.5", procesador Intel Celeron N de hasta 2.79 GHz, 4 GB DDR4, 256 GB de almacenamiento, Bluetooth, teclado retroiluminado, cámara web, Windows 11, azul oscuro,</t>
+  </si>
+  <si>
+    <t>HP Laptop empresarial 255 G10 FHD de 15.6 pulgadas, AMD Ryzen 7 7730U, 32 GB de RAM, SSD PCIe de 1 TB, teclado numérico, cámara web, Wi-Fi 6, HDMI, Windows 11 Pro, negro</t>
+  </si>
+  <si>
+    <t>ASUS Vivobook F1605ZA-AS56 - Computadora portátil WUXGA de 16 pulgadas, memoria de 16 GB, SSD de 512 GB, plata fría</t>
+  </si>
+  <si>
+    <t>298</t>
   </si>
   <si>
     <t>499</t>
   </si>
   <si>
-    <t>389</t>
-  </si>
-  <si>
-    <t>304</t>
-  </si>
-  <si>
-    <t>229</t>
+    <t>349</t>
+  </si>
+  <si>
+    <t>227</t>
   </si>
   <si>
     <t>269</t>
   </si>
   <si>
-    <t>569</t>
+    <t>399</t>
+  </si>
+  <si>
+    <t>279</t>
   </si>
   <si>
     <t>549</t>
   </si>
   <si>
-    <t>861</t>
-  </si>
-  <si>
-    <t>278</t>
-  </si>
-  <si>
-    <t>659</t>
-  </si>
-  <si>
     <t>187</t>
   </si>
   <si>
-    <t>486</t>
-  </si>
-  <si>
-    <t>206</t>
-  </si>
-  <si>
-    <t>449</t>
-  </si>
-  <si>
-    <t>599</t>
-  </si>
-  <si>
-    <t>699</t>
+    <t>215</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>309</t>
+  </si>
+  <si>
+    <t>529</t>
   </si>
   <si>
     <t>239</t>
   </si>
   <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>306</t>
+  </si>
+  <si>
+    <t>429</t>
+  </si>
+  <si>
+    <t>445</t>
+  </si>
+  <si>
     <t>299</t>
   </si>
   <si>
-    <t>165</t>
+    <t>689</t>
   </si>
   <si>
     <t>369</t>
   </si>
   <si>
-    <t>161</t>
+    <t>509</t>
   </si>
   <si>
     <t>179</t>
+  </si>
+  <si>
+    <t>1,281</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>619</t>
   </si>
 </sst>
 </file>
@@ -231,10 +270,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B29" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B35" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" name="Nombre"/>
-    <tableColumn id="2" name="Precio"/>
+    <tableColumn id="1" name="name"/>
+    <tableColumn id="2" name="price"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -525,14 +564,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="201.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="202.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -548,7 +587,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -556,7 +595,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -564,7 +603,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -572,7 +611,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -580,80 +619,83 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="B7" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>38</v>
@@ -661,98 +703,146 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>